<commit_message>
feat: basic app working
moved database folder
generates history of menus
</commit_message>
<xml_diff>
--- a/data/Receitas.xlsx
+++ b/data/Receitas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\gitClones\recipe_planner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9715D4A-3E50-42E8-9A03-7B7788A942BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FE6884-180B-40BF-9274-7329E5CE68CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{774378EC-37D3-4886-97EC-99F503AAA495}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Prato</t>
   </si>
@@ -72,33 +72,6 @@
   </si>
   <si>
     <t>Sab/Dom</t>
-  </si>
-  <si>
-    <t>Arroz, Feijão e Frango com molho de mostarda</t>
-  </si>
-  <si>
-    <t>Arroz de Brócolis com Salmão</t>
-  </si>
-  <si>
-    <t>Arroz de lentilha e lombo acebolado</t>
-  </si>
-  <si>
-    <t>Lasanha à Bolonhesa</t>
-  </si>
-  <si>
-    <t>Arroz com Lentilha e Calabresa</t>
-  </si>
-  <si>
-    <t>Strogonoff de Frango</t>
-  </si>
-  <si>
-    <t>Strogonoff de Carne</t>
-  </si>
-  <si>
-    <t>Risoto de Funghi com File Mingnon</t>
-  </si>
-  <si>
-    <t>Fettuccine Alfredo</t>
   </si>
   <si>
     <t>Nao</t>
@@ -498,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A442F3A7-D6A8-4001-9756-0A68ADEB80AE}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,103 +501,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -689,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -699,7 +579,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>